<commit_message>
Deployed 49684e3 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/en/Manual/source/tab/parameters.xlsx
+++ b/en/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="317">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -584,6 +584,12 @@
     <t xml:space="preserve">Filter already inside of TGS-560-25/50</t>
   </si>
   <si>
+    <t xml:space="preserve">7,8 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 W</t>
+  </si>
+  <si>
     <t xml:space="preserve">11 kW</t>
   </si>
   <si>
@@ -714,9 +720,6 @@
   </si>
   <si>
     <t xml:space="preserve">Losses at maximum output power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 W</t>
   </si>
   <si>
     <t xml:space="preserve">Recommended circuit breaker</t>
@@ -1258,7 +1261,7 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.92"/>
@@ -1478,7 +1481,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -1714,7 +1717,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -1942,7 +1945,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2178,7 +2181,7 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2403,7 +2406,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2623,7 +2626,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -2843,7 +2846,7 @@
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3097,7 +3100,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3351,7 +3354,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3605,7 +3608,7 @@
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
@@ -3859,7 +3862,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4087,7 +4090,7 @@
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4328,7 +4331,7 @@
       <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4558,10 +4561,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4596,7 +4599,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4604,7 +4607,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,7 +4615,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4620,7 +4623,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4628,7 +4631,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4790,11 +4793,11 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -4829,7 +4832,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4845,7 +4848,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4853,7 +4856,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,7 +4864,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5030,7 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5044,91 +5047,91 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5143,7 +5146,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5151,18 +5154,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,12 +5181,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5191,7 +5194,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>130</v>
@@ -5199,18 +5202,18 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -5235,7 +5238,7 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5252,43 +5255,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5297,46 +5300,46 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5351,7 +5354,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5359,18 +5362,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5386,12 +5389,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5399,7 +5402,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>174</v>
@@ -5407,34 +5410,34 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -5459,7 +5462,7 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5484,16 +5487,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -5502,16 +5505,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5520,7 +5523,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -5529,7 +5532,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>159</v>
@@ -5538,16 +5541,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5556,19 +5559,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5583,7 +5586,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5591,18 +5594,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5618,12 +5621,12 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5631,7 +5634,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>163</v>
@@ -5639,15 +5642,15 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>162</v>
@@ -5655,26 +5658,26 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -5699,7 +5702,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5716,28 +5719,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5755,19 +5758,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -5782,28 +5785,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5821,16 +5824,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5838,10 +5841,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5849,15 +5852,15 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -5882,7 +5885,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -5899,28 +5902,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5965,10 +5968,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -5986,10 +5989,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -5998,7 +6001,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -6007,7 +6010,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
@@ -6018,7 +6021,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6067,7 +6070,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -6084,28 +6087,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -6150,10 +6153,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -6171,10 +6174,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -6183,7 +6186,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -6195,7 +6198,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6228,7 +6231,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -6448,7 +6451,7 @@
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
@@ -6463,107 +6466,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6571,16 +6574,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6606,16 +6609,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6641,16 +6644,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6676,16 +6679,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6711,16 +6714,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6746,16 +6749,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6781,16 +6784,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -6816,16 +6819,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -6868,7 +6871,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
@@ -6882,89 +6885,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6984,7 +6987,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -7013,7 +7016,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -7042,7 +7045,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7071,7 +7074,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7100,7 +7103,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7129,7 +7132,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7163,7 +7166,7 @@
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
@@ -7173,44 +7176,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7218,7 +7221,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7232,7 +7235,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>
@@ -7263,7 +7266,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -7510,7 +7513,7 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.65"/>
@@ -7758,11 +7761,11 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8014,7 +8017,7 @@
       <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8242,7 +8245,7 @@
       <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
@@ -8478,7 +8481,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>

</xml_diff>

<commit_message>
Deployed 459651b9 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/en/Manual/source/tab/parameters.xlsx
+++ b/en/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="39"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="339">
   <si>
     <t xml:space="preserve">POWER SUPPLY</t>
   </si>
@@ -987,9 +987,6 @@
   </si>
   <si>
     <t xml:space="preserve"> I&lt;sub&gt;O,max&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Osa č. </t>
   </si>
   <si>
     <t xml:space="preserve"> f&lt;sub&gt;maxSq&lt;/sub&gt;</t>
@@ -9239,8 +9236,8 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9307,10 +9304,10 @@
         <v>308</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9359,7 +9356,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -9388,7 +9385,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -9417,7 +9414,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -9446,7 +9443,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -9475,7 +9472,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -9504,7 +9501,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -9773,7 +9770,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -9790,13 +9787,13 @@
         <v>262</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9804,13 +9801,13 @@
         <v>273</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9824,7 +9821,7 @@
         <v>288</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9894,7 +9891,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>240</v>
@@ -9902,10 +9899,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9935,7 +9932,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>257</v>
@@ -9944,7 +9941,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -9952,66 +9949,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>